<commit_message>
added more ation cat
</commit_message>
<xml_diff>
--- a/AnimeCategories.xlsx
+++ b/AnimeCategories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lin\Documents\Projects\your_anime_sanctuary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FBA2DA-936C-4B4C-87CD-85D700F11C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D806C07-2EFA-4E2E-BF00-B82DF18CA60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AB93213C-F751-41C9-8D14-BFF51B28E666}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AB93213C-F751-41C9-8D14-BFF51B28E666}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -249,9 +249,6 @@
     <t>Plastic Memories</t>
   </si>
   <si>
-    <t>3d_kanojo</t>
-  </si>
-  <si>
     <t>Bananafish</t>
   </si>
   <si>
@@ -283,6 +280,9 @@
   </si>
   <si>
     <t>Tokyo Magnitude 8.0</t>
+  </si>
+  <si>
+    <t>3D_kanojo</t>
   </si>
 </sst>
 </file>
@@ -709,7 +709,7 @@
   <dimension ref="B2:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,7 +751,7 @@
         <v>59</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -780,7 +780,7 @@
         <v>60</v>
       </c>
       <c r="J4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -788,7 +788,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
@@ -814,7 +814,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -869,16 +869,16 @@
         <v>5</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>28</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="G8" t="s">
         <v>35</v>
@@ -899,7 +899,7 @@
         <v>68</v>
       </c>
       <c r="D9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E9" t="s">
         <v>29</v>
@@ -949,7 +949,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E11" t="s">
         <v>42</v>
@@ -972,10 +972,10 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>70</v>
@@ -1018,7 +1018,7 @@
         <v>18</v>
       </c>
       <c r="E14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K14" s="9"/>
     </row>

</xml_diff>

<commit_message>
added api + SOL
</commit_message>
<xml_diff>
--- a/AnimeCategories.xlsx
+++ b/AnimeCategories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lin\Documents\Projects\your_anime_sanctuary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557D243D-BA6B-45D4-8579-406DD262CC79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3547D937-2477-4DE2-9A84-652EB40C9DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AB93213C-F751-41C9-8D14-BFF51B28E666}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AB93213C-F751-41C9-8D14-BFF51B28E666}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="90">
   <si>
     <t>Action</t>
   </si>
@@ -198,15 +198,9 @@
     <t>No Game no Life</t>
   </si>
   <si>
-    <t>Horimiya</t>
-  </si>
-  <si>
     <t>Ano Hana</t>
   </si>
   <si>
-    <t>Your Lie in April</t>
-  </si>
-  <si>
     <t>Welcome to the NHK</t>
   </si>
   <si>
@@ -301,6 +295,15 @@
   </si>
   <si>
     <t>Cowboy</t>
+  </si>
+  <si>
+    <t>Classroom of the Elite</t>
+  </si>
+  <si>
+    <t>Wotaku</t>
+  </si>
+  <si>
+    <t>GTO</t>
   </si>
 </sst>
 </file>
@@ -385,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -415,6 +418,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,17 +735,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A573A0D0-7F4A-4CBF-BC79-C9335C9C6D9E}">
   <dimension ref="B2:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="28.140625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="10" customWidth="1"/>
     <col min="5" max="5" width="20" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="35.42578125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" style="10" customWidth="1"/>
     <col min="8" max="8" width="22.140625" customWidth="1"/>
     <col min="9" max="9" width="20.28515625" customWidth="1"/>
     <col min="10" max="10" width="18.7109375" customWidth="1"/>
@@ -755,7 +759,7 @@
       <c r="C3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="11" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="11" t="s">
@@ -764,17 +768,17 @@
       <c r="F3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="11" t="s">
         <v>5</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -784,23 +788,23 @@
       <c r="C4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="10" t="s">
         <v>23</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>43</v>
       </c>
       <c r="I4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -808,9 +812,9 @@
         <v>2</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="10" t="s">
@@ -819,14 +823,14 @@
       <c r="F5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="10" t="s">
         <v>37</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>44</v>
       </c>
       <c r="I5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -834,9 +838,9 @@
         <v>3</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="10" t="s">
@@ -845,7 +849,7 @@
       <c r="F6" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="10" t="s">
         <v>40</v>
       </c>
       <c r="H6" s="6" t="s">
@@ -862,7 +866,7 @@
       <c r="C7" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="10" t="s">
         <v>16</v>
       </c>
       <c r="E7" s="10" t="s">
@@ -871,14 +875,14 @@
       <c r="F7" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="10" t="s">
         <v>53</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>46</v>
       </c>
       <c r="I7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>20</v>
@@ -889,16 +893,19 @@
         <v>5</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" t="s">
-        <v>79</v>
+        <v>69</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>77</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>28</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>87</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>47</v>
@@ -913,10 +920,10 @@
         <v>6</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" t="s">
-        <v>80</v>
+        <v>66</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>78</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>29</v>
@@ -924,14 +931,11 @@
       <c r="F9" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="G9" t="s">
-        <v>54</v>
-      </c>
       <c r="H9" s="6" t="s">
         <v>48</v>
       </c>
       <c r="I9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>21</v>
@@ -944,21 +948,21 @@
       <c r="C10" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>41</v>
       </c>
       <c r="F10" s="13"/>
-      <c r="G10" t="s">
-        <v>55</v>
+      <c r="G10" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>49</v>
       </c>
       <c r="I10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -966,10 +970,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D11" t="s">
-        <v>83</v>
+        <v>75</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>81</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>42</v>
@@ -977,14 +981,11 @@
       <c r="F11" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="G11" t="s">
-        <v>56</v>
-      </c>
       <c r="H11" s="6" t="s">
         <v>50</v>
       </c>
       <c r="I11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -992,25 +993,25 @@
         <v>9</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="D12" t="s">
-        <v>86</v>
+        <v>76</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>84</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="G12" t="s">
-        <v>57</v>
+        <v>68</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>55</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>51</v>
       </c>
       <c r="I12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K12" s="4"/>
     </row>
@@ -1019,19 +1020,19 @@
         <v>10</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" t="s">
-        <v>87</v>
+        <v>60</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>85</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F13" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G13" t="s">
-        <v>58</v>
+      <c r="G13" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>52</v>
@@ -1043,27 +1044,33 @@
       <c r="C14" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D14" t="s">
-        <v>88</v>
+      <c r="D14" s="10" t="s">
+        <v>86</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F14" s="13" t="s">
         <v>35</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>89</v>
       </c>
       <c r="K14" s="8"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="F15" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="F16" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
@@ -1072,7 +1079,7 @@
         <v>30</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
@@ -1081,7 +1088,7 @@
         <v>10</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
@@ -1106,5 +1113,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>